<commit_message>
some questions by 9/10
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7C2987B9-FBE6-4253-819F-8569EA94A1D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Test/Train seems relatively well balanced AP vs PA</t>
   </si>
@@ -38,17 +38,49 @@
   </si>
   <si>
     <t>Different pixel spacing AP vs PA (probably due to different location of patient relative to imaging machine)</t>
+  </si>
+  <si>
+    <r>
+      <t>pixel spacing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对分析的影响</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般图像分析的方法:CNN,DNN?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像需要做什么样的data preprocessing吗? 例如pixel normalization之类的?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>要不要先做分类分析 然后再具体分析+框</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>activation function等之类的需要什么注意的?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -57,6 +89,20 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -364,50 +410,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="94.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="14.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="14.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="14.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="14.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update from company laptop
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Test/Train seems relatively well balanced AP vs PA</t>
   </si>
@@ -60,15 +60,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>图像需要做什么样的data preprocessing吗? 例如pixel normalization之类的?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>要不要先做分类分析 然后再具体分析+框</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>activation function等之类的需要什么注意的?</t>
+    <t>activation function等之类的需要什么注意的? (sigmoid, Relu,tanh等?)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像需要做什么样的data preprocessing吗? 例如color standardization, b/w pixel rate, pic rotation, pic zoom in/out; pixel normalization之类的?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNN推荐的python的包? Keras,mxnet,sklearn-theano,Mask-RCNN等</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>敏感区域系数百分比</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>整个图片的比较</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>keras比较好上手 但是比较简练</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tensorflow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>整个图的分割 vs 权重的输出 vs 其他的输出</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>luna的肺结节比赛?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -461,10 +489,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -481,33 +509,24 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
@@ -533,6 +552,9 @@
       <c r="A10">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
@@ -543,16 +565,25 @@
       <c r="A12">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
         <v>14</v>
       </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
@@ -564,23 +595,54 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "update from company laptop"
This reverts commit 48d03fa345d61d8db5eaef44877b2dc4f47e3b85.
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Test/Train seems relatively well balanced AP vs PA</t>
   </si>
@@ -60,43 +60,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>图像需要做什么样的data preprocessing吗? 例如pixel normalization之类的?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>要不要先做分类分析 然后再具体分析+框</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>activation function等之类的需要什么注意的? (sigmoid, Relu,tanh等?)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>图像需要做什么样的data preprocessing吗? 例如color standardization, b/w pixel rate, pic rotation, pic zoom in/out; pixel normalization之类的?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CNN推荐的python的包? Keras,mxnet,sklearn-theano,Mask-RCNN等</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>敏感区域系数百分比</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>整个图片的比较</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>keras比较好上手 但是比较简练</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tensorflow</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>整个图的分割 vs 权重的输出 vs 其他的输出</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>luna的肺结节比赛?</t>
+    <t>activation function等之类的需要什么注意的?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -489,10 +461,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -509,24 +481,33 @@
       <c r="A2">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
@@ -552,9 +533,6 @@
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
@@ -565,25 +543,16 @@
       <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
@@ -595,54 +564,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:1">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:1">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:1">
       <c r="A19">
         <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="B25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="B26" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>